<commit_message>
Actualizando los mejores resultados de k 10
</commit_message>
<xml_diff>
--- a/results/best-results-k10.xlsx
+++ b/results/best-results-k10.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Resultados_rprecision_mostpop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marta\Documents\Doctorado\Experimentos\Aplicación TFM a MovieLens\MovieLens_Experiment_9010\Experimentos 9010 random testset\Graph-Recommendations\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CACF47-CBB9-43BB-AF1D-707A6A6E6B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="50% - k = 10" sheetId="37" r:id="rId1"/>
@@ -26,11 +27,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - decisionTree_9010_unos_ceros" description="Conexión a la consulta 'decisionTree_9010_unos_ceros' en el libro." type="5" refreshedVersion="6" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - decisionTree_9010_unos_ceros" description="Conexión a la consulta 'decisionTree_9010_unos_ceros' en el libro." type="5" refreshedVersion="6" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=decisionTree_9010_unos_ceros;Extended Properties=&quot;&quot;" command="SELECT * FROM [decisionTree_9010_unos_ceros]"/>
   </connection>
-  <connection id="2" keepAlive="1" name="Consulta - neural_networks_9010_UnosCeros_most_popular" description="Conexión a la consulta 'neural_networks_9010_UnosCeros_most_popular' en el libro." type="5" refreshedVersion="6" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Consulta - neural_networks_9010_UnosCeros_most_popular" description="Conexión a la consulta 'neural_networks_9010_UnosCeros_most_popular' en el libro." type="5" refreshedVersion="6" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=neural_networks_9010_UnosCeros_most_popular;Extended Properties=&quot;&quot;" command="SELECT * FROM [neural_networks_9010_UnosCeros_most_popular]"/>
   </connection>
 </connections>
@@ -135,7 +136,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +226,7 @@
     <xf numFmtId="2" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,11 +510,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,10 +735,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="11">
-        <v>0.665116279069768</v>
+        <v>0.65891472868217005</v>
       </c>
       <c r="E15" s="11">
-        <v>0.66537269793083698</v>
+        <v>0.65547946885156105</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -951,15 +952,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1186,10 +1188,10 @@
         <v>0.99734042553191404</v>
       </c>
       <c r="D15" s="11">
-        <v>0.59388297872340401</v>
+        <v>0.59255319148936103</v>
       </c>
       <c r="E15" s="11">
-        <v>0.6264826631007</v>
+        <v>0.62396135535997799</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1418,11 +1420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1640,13 +1642,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="11">
-        <v>0.97826086956521696</v>
+        <v>0.97491638795986602</v>
       </c>
       <c r="D15" s="11">
-        <v>0.46070234113712299</v>
+        <v>0.459197324414715</v>
       </c>
       <c r="E15" s="11">
-        <v>0.53600125746987803</v>
+        <v>0.536023698796667</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -1852,10 +1854,10 @@
         <v>0.993311036789297</v>
       </c>
       <c r="D31" s="11">
-        <v>0.467391304347825</v>
+        <v>0.467892976588628</v>
       </c>
       <c r="E31" s="11">
-        <v>0.11043601975876199</v>
+        <v>0.110017959558093</v>
       </c>
     </row>
   </sheetData>

</xml_diff>